<commit_message>
Made changes to NuMAD excel example file to be compatable with updated version of xlsread.m
</commit_message>
<xml_diff>
--- a/examples/numadGUI/NuMADforExcel/NuMAD.xlsx
+++ b/examples/numadGUI/NuMADforExcel/NuMAD.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AFF988-4589-4769-B57D-FF2E47DCAF7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="31410" yWindow="4530" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="2" r:id="rId1"/>
     <sheet name="Geometry" sheetId="1" r:id="rId2"/>
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="85">
   <si>
     <t>Twist (deg)</t>
   </si>
@@ -268,12 +279,15 @@
   </si>
   <si>
     <t>E22 (not used for isotropic)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,6 +344,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -377,7 +394,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,9 +427,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,6 +479,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,23 +671,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="145.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="17" max="17" width="145.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>15</v>
       </c>
@@ -683,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -724,7 +778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -755,7 +809,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>A4+1</f>
         <v>2</v>
@@ -787,7 +841,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ref="A6:A8" si="0">A5+1</f>
         <v>3</v>
@@ -825,7 +879,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -857,7 +911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -895,32 +949,32 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -933,7 +987,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -941,26 +995,26 @@
       <selection pane="topRight" activeCell="AJ31" sqref="AJ31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" customWidth="1"/>
-    <col min="25" max="32" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.109375" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" customWidth="1"/>
+    <col min="25" max="32" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -1058,7 +1112,7 @@
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>32</v>
       </c>
@@ -1113,7 +1167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1223,7 +1277,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1329,7 +1383,7 @@
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1403,7 +1457,7 @@
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1460,7 +1514,7 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1517,7 +1571,7 @@
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1574,7 +1628,7 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1640,7 +1694,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1706,7 +1760,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1775,7 +1829,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1863,7 +1917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1921,7 +1975,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1979,7 +2033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2037,7 +2091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2095,7 +2149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2176,7 +2230,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2233,7 +2287,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2290,7 +2344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2347,7 +2401,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2404,7 +2458,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2489,7 +2543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2546,7 +2600,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2603,7 +2657,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2660,7 +2714,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2717,7 +2771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2823,7 +2877,7 @@
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
@@ -2842,7 +2896,7 @@
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
@@ -2861,7 +2915,7 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
@@ -2880,7 +2934,7 @@
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
@@ -2897,7 +2951,7 @@
       <c r="AL31" s="1"/>
       <c r="AN31" s="1"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
@@ -2913,7 +2967,7 @@
       <c r="AL32" s="1"/>
       <c r="AN32" s="1"/>
     </row>
-    <row r="33" spans="24:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="24:40" x14ac:dyDescent="0.3">
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
@@ -2929,7 +2983,7 @@
       <c r="AL33" s="1"/>
       <c r="AN33" s="1"/>
     </row>
-    <row r="34" spans="24:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="24:40" x14ac:dyDescent="0.3">
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
@@ -2945,7 +2999,7 @@
       <c r="AL34" s="1"/>
       <c r="AN34" s="1"/>
     </row>
-    <row r="35" spans="24:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="24:40" x14ac:dyDescent="0.3">
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
@@ -2961,14 +3015,14 @@
       <c r="AL35" s="1"/>
       <c r="AN35" s="1"/>
     </row>
-    <row r="41" spans="24:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="24:40" x14ac:dyDescent="0.3">
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="B2:G52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G52">
     <sortCondition ref="B2:B52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2977,19 +3031,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>

</xml_diff>